<commit_message>
Prepared External Data for merging
</commit_message>
<xml_diff>
--- a/ExternalData/GDPGrowth.xlsx
+++ b/ExternalData/GDPGrowth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/fce19_ic_ac_uk/Documents/Programming/ShellDatathon/ExternalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_AD4DB114E441178AC67DF4B42615F688683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A2E24F5-92F8-4BE5-BF52-EF5DBB0D26F3}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_AD4DB114E441178AC67DF4B42615F688683EDF19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC7EB525-D3B0-4C9E-A00F-C9EE8AF8C0C0}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2964" yWindow="2964" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,75 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t>elease Date</t>
-  </si>
-  <si>
-    <t>Dec 02, 2019 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 02, 2019 (Q2)</t>
-  </si>
-  <si>
-    <t>May 31, 2019 (Q1)</t>
-  </si>
-  <si>
-    <t>Mar 11, 2019 (Q4)</t>
-  </si>
-  <si>
-    <t>Dec 10, 2018 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 10, 2018 (Q2)</t>
-  </si>
-  <si>
-    <t>Jun 11, 2018 (Q1)</t>
-  </si>
-  <si>
-    <t>Mar 29, 2018 (Q4)</t>
-  </si>
-  <si>
-    <t>Dec 11, 2017 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 11, 2017 (Q2)</t>
-  </si>
-  <si>
-    <t>Jun 12, 2017 (Q1)</t>
-  </si>
-  <si>
-    <t>Mar 31, 2017 (Q4)</t>
-  </si>
-  <si>
-    <t>Dec 12, 2016 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 09, 2016 (Q2)</t>
-  </si>
-  <si>
-    <t>Jun 10, 2016 (Q1)</t>
-  </si>
-  <si>
-    <t>Mar 31, 2016 (Q4)</t>
-  </si>
-  <si>
-    <t>Dec 10, 2015 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 10, 2015 (Q2)</t>
-  </si>
-  <si>
-    <t>Jun 10, 2015 (Q1)</t>
-  </si>
-  <si>
-    <t>Mar 31, 2015 (Q4)</t>
-  </si>
-  <si>
-    <t>Dec 10, 2014 (Q3)</t>
-  </si>
-  <si>
-    <t>Sep 10, 2014 (Q2)</t>
-  </si>
-  <si>
     <t>Jun 10, 2014</t>
   </si>
   <si>
@@ -106,6 +37,75 @@
   </si>
   <si>
     <t>GDP Growth</t>
+  </si>
+  <si>
+    <t>Release Date</t>
+  </si>
+  <si>
+    <t>Dec 02, 2019</t>
+  </si>
+  <si>
+    <t>Sep 02, 2019</t>
+  </si>
+  <si>
+    <t>May 31, 2019</t>
+  </si>
+  <si>
+    <t>Mar 11, 2019</t>
+  </si>
+  <si>
+    <t>Dec 10, 2018</t>
+  </si>
+  <si>
+    <t>Sep 10, 2018</t>
+  </si>
+  <si>
+    <t>Jun 11, 2018</t>
+  </si>
+  <si>
+    <t>Mar 29, 2018</t>
+  </si>
+  <si>
+    <t>Dec 11, 2017</t>
+  </si>
+  <si>
+    <t>Sep 11, 2017</t>
+  </si>
+  <si>
+    <t>Jun 12, 2017</t>
+  </si>
+  <si>
+    <t>Mar 31, 2017</t>
+  </si>
+  <si>
+    <t>Dec 12, 2016</t>
+  </si>
+  <si>
+    <t>Sep 09, 2016</t>
+  </si>
+  <si>
+    <t>Jun 10, 2016</t>
+  </si>
+  <si>
+    <t>Mar 31, 2016</t>
+  </si>
+  <si>
+    <t>Dec 10, 2015</t>
+  </si>
+  <si>
+    <t>Sep 10, 2015</t>
+  </si>
+  <si>
+    <t>Jun 10, 2015</t>
+  </si>
+  <si>
+    <t>Mar 31, 2015</t>
+  </si>
+  <si>
+    <t>Dec 10, 2014</t>
+  </si>
+  <si>
+    <t>Sep 10, 2014</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -493,15 +493,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4">
         <v>8.9999999999999993E-3</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
         <v>-1.4999999999999999E-2</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>-2.5999999999999999E-2</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>-0.03</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4">
         <v>1.6E-2</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6">
         <v>5.1999999999999998E-2</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5">
         <v>7.3999999999999996E-2</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5">
         <v>7.2999999999999995E-2</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="5">
         <v>0.111</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
         <v>5.0999999999999997E-2</v>
@@ -581,7 +581,7 @@
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5">
         <v>0.05</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B13" s="5">
         <v>3.5000000000000003E-2</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4">
         <v>-1.7999999999999999E-2</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15" s="4">
         <v>3.1E-2</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5">
         <v>4.8000000000000001E-2</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" s="5">
         <v>5.7000000000000002E-2</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="5">
         <v>0.04</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5">
         <v>3.7999999999999999E-2</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" s="5">
         <v>2.3E-2</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B21" s="5">
         <v>2.5999999999999999E-2</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="4">
         <v>1.7000000000000001E-2</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="4">
         <v>2.1000000000000001E-2</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B24" s="6">
         <v>4.2999999999999997E-2</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B25" s="5">
         <v>4.3999999999999997E-2</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B26" s="5">
         <v>4.3999999999999997E-2</v>

</xml_diff>